<commit_message>
Remove attribute redefinitions from Micrograph class
Removed redefinitions of pixel_size, defocus, dose, and astigmatism
from the Micrograph class. These attributes are now inherited from
parent classes Image and Image2D, eliminating conflicts and ambiguity.

Co-authored-by: cmungall <50745+cmungall@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/assets/excel/lambda-ber-schema.xlsx
+++ b/assets/excel/lambda-ber-schema.xlsx
@@ -35,23 +35,30 @@
     <sheet name="Image" sheetId="26" state="visible" r:id="rId26"/>
     <sheet name="Image2D" sheetId="27" state="visible" r:id="rId27"/>
     <sheet name="Image3D" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="FTIRImage" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="FluorescenceImage" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="OpticalImage" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="XRFImage" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="ImageFeature" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="OntologyTerm" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="MolecularComposition" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="BufferComposition" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="StorageConditions" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="CryoEMPreparation" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="CrystallizationConditions" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="XRayPreparation" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="SAXSPreparation" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="ExperimentalConditions" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="DataCollectionStrategy" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="QualityMetrics" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="ComputeResources" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="Movie" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="Micrograph" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="FTIRImage" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="FluorescenceImage" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="OpticalImage" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="XRFImage" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="ImageFeature" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="OntologyTerm" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="MolecularComposition" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="BufferComposition" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="StorageConditions" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="CryoEMPreparation" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="CrystallizationConditions" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="XRayPreparation" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="SAXSPreparation" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="ExperimentalConditions" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="DataCollectionStrategy" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="QualityMetrics" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="ComputeResources" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="MotionCorrectionParameters" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="CTFEstimationParameters" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="ParticlePickingParameters" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="RefinementParameters" sheetId="51" state="visible" r:id="rId51"/>
+    <sheet name="FSCCurve" sheetId="52" state="visible" r:id="rId52"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1891,7 +1898,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:AG1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1942,40 +1949,125 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>cs</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>c2_aperture</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>objective_aperture</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>phase_plate_type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>energy_filter_present</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>energy_filter_make</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>energy_filter_model</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>energy_filter_slit_width</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>detector_position</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>detector_mode</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>pixel_size_physical</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>microscope_software</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>microscope_software_version</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>spotsize</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>gunlens</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>imaging_mode</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>tem_beam_diameter</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
           <t>instrument_code</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>manufacturer</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>model</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>installation_date</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>current_status</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -1986,7 +2078,7 @@
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"direct_electron,ccd,cmos,hybrid_pixel,eiger,pilatus,rayonix,adsc,mar"</formula1>
     </dataValidation>
-    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="AD2:AD1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"operational,maintenance,offline,commissioning"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2223,7 +2315,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AT1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2294,70 +2386,170 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
+          <t>magnification</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>calibrated_pixel_size</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>camera_binning</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>exposure_time_per_frame</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>frames_per_movie</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>total_exposure_time</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>total_dose</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>dose_rate</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>defocus_target</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>defocus_range_min</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>defocus_range_max</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>defocus_range_increment</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>astigmatism_target</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>coma</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>stage_tilt</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>autoloader_slot</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>shots_per_hole</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>holes_per_group</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>acquisition_software</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>acquisition_software_version</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
           <t>wavelength</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>oscillation_angle</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>start_angle</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>number_of_images</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>beam_center_x</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>beam_center_y</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>detector_distance</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>pixel_size_x</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>pixel_size_y</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>total_rotation</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>beamline</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -2385,7 +2577,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BC1"/>
+  <dimension ref="A1:BH1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2651,30 +2843,52 @@
       </c>
       <c r="AZ1" t="inlineStr">
         <is>
+          <t>motion_correction_params</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>ctf_estimation_params</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>particle_picking_params</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>refinement_params</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>fsc_curve</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
           <t>output_files</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"motion_correction,ctf_estimation,particle_picking,classification_2d,classification_3d,refinement,model_building,phasing,integration,scaling,saxs_analysis,em_2d_classification,mass_spec_deconvolution"</formula1>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"molecular_replacement,sad,mad,sir,mir,siras,miras,fragile_mr"</formula1>
     </dataValidation>
@@ -2689,7 +2903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2735,15 +2949,30 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>storage_uri</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>related_entity</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>file_role</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -2752,10 +2981,10 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"mrc,tiff,hdf5,star,pdb,mmcif,mtz,cbf,cbf_zst,img,h5,ascii,thermo_raw,zip,gz"</formula1>
+      <formula1>"mrc,tiff,hdf5,star,pdb,mmcif,mtz,cbf,cbf_zst,img,h5,ascii,thermo_raw,zip,mrcs,eer,cs,json,csv,ccp4,gz"</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"micrograph,diffraction,scattering,particles,volume,model,metadata,raw_data,processed_data"</formula1>
+      <formula1>"micrograph,diffraction,scattering,particles,volume,model,metadata,raw_data,processed_data,movie,motion_corrected,ctf_estimation,particle_coordinates,class_averages,fsc_curve,map_half,validation_report"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3006,7 +3235,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3017,85 +3246,135 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>wavenumber_min</t>
+          <t>frames</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>wavenumber_max</t>
+          <t>super_resolution</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>spectral_resolution</t>
+          <t>pixel_size_unbinned</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>number_of_scans</t>
+          <t>timestamp</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>apodization_function</t>
+          <t>stage_position_x</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>molecular_signatures</t>
+          <t>stage_position_y</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>background_correction</t>
+          <t>stage_position_z</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>nominal_defocus</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>dose_per_frame</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>beam_shift_x</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>beam_shift_y</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>ice_thickness_estimate</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>grid_square_id</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>hole_id</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>acquisition_group</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>defocus</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>astigmatism</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>file_name</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>acquisition_date</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>pixel_size</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>dimensions_x</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>dimensions_y</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>exposure_time</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>dose</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -3257,6 +3536,223 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:R1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>origin_movie_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>defocus_u</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>defocus_v</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>astigmatism_angle</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>resolution_fit_limit</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>ctf_quality_score</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>defocus</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>astigmatism</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>file_name</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>acquisition_date</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>dimensions_x</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>dimensions_y</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>exposure_time</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>dose</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>wavenumber_min</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>wavenumber_max</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>spectral_resolution</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>number_of_scans</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>apodization_function</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>molecular_signatures</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>background_correction</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>file_name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>acquisition_date</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>dimensions_x</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>dimensions_y</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>exposure_time</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>dose</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3377,7 +3873,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3493,7 +3989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3619,7 +4115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3650,7 +4146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3701,7 +4197,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3742,7 +4238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3783,7 +4279,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3828,181 +4324,6 @@
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"celsius,kelvin,fahrenheit"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>grid_type</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>support_film</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>hole_size</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>vitrification_method</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>blot_time</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>blot_force</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>humidity_percentage</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>chamber_temperature</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>plasma_treatment</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"c_flat,quantifoil,lacey_carbon,ultrathin_carbon,gold"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"plunge_freezing,high_pressure_freezing,slam_freezing"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:N1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>method</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>crystallization_conditions</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>drop_volume</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>protein_concentration</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>crystal_size_um</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>cryo_protectant</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>crystal_id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>screen_name</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>temperature_c</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>drop_ratio_protein_to_reservoir</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>reservoir_volume_ul</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>seeding_type</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>seed_stock_dilution</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"vapor_diffusion_hanging,vapor_diffusion_sitting,batch,microbatch,lcp,dialysis,free_interface_diffusion"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4112,6 +4433,246 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:W1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>grid_type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>support_film</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>hole_size</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>vitrification_method</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>blot_time</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>blot_force</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>humidity_percentage</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>chamber_temperature</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>grid_material</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>glow_discharge_applied</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>glow_discharge_time</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>glow_discharge_current</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>glow_discharge_atmosphere</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>glow_discharge_pressure</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>vitrification_instrument</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>blot_number</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>wait_time</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>blotter_height</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>blotter_setting</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>sample_applied_volume</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>ethane_temperature</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>plasma_treatment</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"c_flat,quantifoil,lacey_carbon,ultrathin_carbon,gold"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"plunge_freezing,high_pressure_freezing,slam_freezing"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>method</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>crystallization_conditions</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>drop_volume</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>protein_concentration</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>crystal_size_um</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>cryo_protectant</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>crystal_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>screen_name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>temperature_c</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>drop_ratio_protein_to_reservoir</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>reservoir_volume_ul</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>seeding_type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>seed_stock_dilution</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"vapor_diffusion_hanging,vapor_diffusion_sitting,batch,microbatch,lcp,dialysis,free_interface_diffusion"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4262,7 +4823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4313,7 +4874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4369,7 +4930,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4490,7 +5051,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4676,7 +5237,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4712,6 +5273,128 @@
         </is>
       </c>
       <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>patch_size</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>binning</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dose_weighting</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>bfactor_dose_weighting</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>anisotropic_correction</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>frame_grouping</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_binning</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>drift_total</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>defocus_search_min</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>defocus_search_max</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>defocus_step</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>amplitude_contrast</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>cs</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>voltage</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -4865,6 +5548,164 @@
       <formula1>"experimental,predicted,inferred,literature,author_statement,curator_inference"</formula1>
     </dataValidation>
   </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>picking_method</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>box_size</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>power_score</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>ncc_score</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>model_file</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>symmetry</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>box_size</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>gold_standard</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>split_strategy</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>resolution_0_143</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>resolution_0_5</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>map_sharpening_bfactor</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>resolution_angstrom</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>fsc_value</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add ImagingModeEnum for controlled vocabulary in imaging_mode attribute
Co-authored-by: cmungall <50745+cmungall@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/assets/excel/lambda-ber-schema.xlsx
+++ b/assets/excel/lambda-ber-schema.xlsx
@@ -35,23 +35,30 @@
     <sheet name="Image" sheetId="26" state="visible" r:id="rId26"/>
     <sheet name="Image2D" sheetId="27" state="visible" r:id="rId27"/>
     <sheet name="Image3D" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="FTIRImage" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="FluorescenceImage" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="OpticalImage" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="XRFImage" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="ImageFeature" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="OntologyTerm" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="MolecularComposition" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="BufferComposition" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="StorageConditions" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="CryoEMPreparation" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="CrystallizationConditions" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="XRayPreparation" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="SAXSPreparation" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="ExperimentalConditions" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="DataCollectionStrategy" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="QualityMetrics" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="ComputeResources" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="Movie" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="Micrograph" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="FTIRImage" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="FluorescenceImage" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="OpticalImage" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="XRFImage" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="ImageFeature" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="OntologyTerm" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="MolecularComposition" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="BufferComposition" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="StorageConditions" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="CryoEMPreparation" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="CrystallizationConditions" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="XRayPreparation" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="SAXSPreparation" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="ExperimentalConditions" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="DataCollectionStrategy" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="QualityMetrics" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="ComputeResources" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="MotionCorrectionParameters" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="CTFEstimationParameters" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="ParticlePickingParameters" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="RefinementParameters" sheetId="51" state="visible" r:id="rId51"/>
+    <sheet name="FSCCurve" sheetId="52" state="visible" r:id="rId52"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1891,7 +1898,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:AG1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1942,51 +1949,139 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>cs</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>c2_aperture</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>objective_aperture</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>phase_plate_type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>energy_filter_present</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>energy_filter_make</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>energy_filter_model</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>energy_filter_slit_width</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>detector_position</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>detector_mode</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>pixel_size_physical</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>microscope_software</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>microscope_software_version</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>spotsize</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>gunlens</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>imaging_mode</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>tem_beam_diameter</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
           <t>instrument_code</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>manufacturer</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>model</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>installation_date</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>current_status</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"direct_electron,ccd,cmos,hybrid_pixel,eiger,pilatus,rayonix,adsc,mar"</formula1>
     </dataValidation>
-    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="X2:X1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"EFTEM,TEM,STEM"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AD2:AD1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"operational,maintenance,offline,commissioning"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2223,7 +2318,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AT1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2294,70 +2389,170 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
+          <t>magnification</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>calibrated_pixel_size</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>camera_binning</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>exposure_time_per_frame</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>frames_per_movie</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>total_exposure_time</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>total_dose</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>dose_rate</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>defocus_target</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>defocus_range_min</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>defocus_range_max</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>defocus_range_increment</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>astigmatism_target</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>coma</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>stage_tilt</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>autoloader_slot</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>shots_per_hole</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>holes_per_group</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>acquisition_software</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>acquisition_software_version</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
           <t>wavelength</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>oscillation_angle</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>start_angle</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>number_of_images</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>beam_center_x</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>beam_center_y</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>detector_distance</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>pixel_size_x</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>pixel_size_y</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>total_rotation</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>beamline</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -2385,7 +2580,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BC1"/>
+  <dimension ref="A1:BH1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2651,30 +2846,52 @@
       </c>
       <c r="AZ1" t="inlineStr">
         <is>
+          <t>motion_correction_params</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>ctf_estimation_params</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>particle_picking_params</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>refinement_params</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>fsc_curve</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
           <t>output_files</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"motion_correction,ctf_estimation,particle_picking,classification_2d,classification_3d,refinement,model_building,phasing,integration,scaling,saxs_analysis,em_2d_classification,mass_spec_deconvolution"</formula1>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"molecular_replacement,sad,mad,sir,mir,siras,miras,fragile_mr"</formula1>
     </dataValidation>
@@ -2689,7 +2906,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2735,15 +2952,30 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>storage_uri</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>related_entity</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>file_role</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -2752,10 +2984,10 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"mrc,tiff,hdf5,star,pdb,mmcif,mtz,cbf,cbf_zst,img,h5,ascii,thermo_raw,zip,gz"</formula1>
+      <formula1>"mrc,tiff,hdf5,star,pdb,mmcif,mtz,cbf,cbf_zst,img,h5,ascii,thermo_raw,zip,mrcs,eer,cs,json,csv,ccp4,gz"</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"micrograph,diffraction,scattering,particles,volume,model,metadata,raw_data,processed_data"</formula1>
+      <formula1>"micrograph,diffraction,scattering,particles,volume,model,metadata,raw_data,processed_data,movie,motion_corrected,ctf_estimation,particle_coordinates,class_averages,fsc_curve,map_half,validation_report"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3006,7 +3238,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3017,85 +3249,135 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>wavenumber_min</t>
+          <t>frames</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>wavenumber_max</t>
+          <t>super_resolution</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>spectral_resolution</t>
+          <t>pixel_size_unbinned</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>number_of_scans</t>
+          <t>timestamp</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>apodization_function</t>
+          <t>stage_position_x</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>molecular_signatures</t>
+          <t>stage_position_y</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>background_correction</t>
+          <t>stage_position_z</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>nominal_defocus</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>dose_per_frame</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>beam_shift_x</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>beam_shift_y</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>ice_thickness_estimate</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>grid_square_id</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>hole_id</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>acquisition_group</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>defocus</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>astigmatism</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>file_name</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>acquisition_date</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>pixel_size</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>dimensions_x</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>dimensions_y</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>exposure_time</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>dose</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -3257,6 +3539,223 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:R1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>defocus</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dose</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>origin_movie_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>defocus_u</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>defocus_v</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>astigmatism</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>astigmatism_angle</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>resolution_fit_limit</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>ctf_quality_score</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>file_name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>acquisition_date</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>dimensions_x</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>dimensions_y</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>exposure_time</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>wavenumber_min</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>wavenumber_max</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>spectral_resolution</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>number_of_scans</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>apodization_function</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>molecular_signatures</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>background_correction</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>file_name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>acquisition_date</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>dimensions_x</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>dimensions_y</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>exposure_time</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>dose</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3377,7 +3876,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3493,7 +3992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3619,7 +4118,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3650,7 +4149,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3701,7 +4200,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3742,7 +4241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3783,7 +4282,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3828,181 +4327,6 @@
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"celsius,kelvin,fahrenheit"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>grid_type</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>support_film</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>hole_size</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>vitrification_method</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>blot_time</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>blot_force</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>humidity_percentage</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>chamber_temperature</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>plasma_treatment</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"c_flat,quantifoil,lacey_carbon,ultrathin_carbon,gold"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"plunge_freezing,high_pressure_freezing,slam_freezing"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:N1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>method</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>crystallization_conditions</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>drop_volume</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>protein_concentration</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>crystal_size_um</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>cryo_protectant</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>crystal_id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>screen_name</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>temperature_c</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>drop_ratio_protein_to_reservoir</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>reservoir_volume_ul</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>seeding_type</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>seed_stock_dilution</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"vapor_diffusion_hanging,vapor_diffusion_sitting,batch,microbatch,lcp,dialysis,free_interface_diffusion"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4112,6 +4436,246 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:W1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>grid_type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>support_film</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>hole_size</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>vitrification_method</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>blot_time</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>blot_force</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>humidity_percentage</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>chamber_temperature</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>grid_material</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>glow_discharge_applied</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>glow_discharge_time</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>glow_discharge_current</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>glow_discharge_atmosphere</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>glow_discharge_pressure</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>vitrification_instrument</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>blot_number</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>wait_time</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>blotter_height</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>blotter_setting</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>sample_applied_volume</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>ethane_temperature</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>plasma_treatment</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"c_flat,quantifoil,lacey_carbon,ultrathin_carbon,gold"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"plunge_freezing,high_pressure_freezing,slam_freezing"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>method</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>crystallization_conditions</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>drop_volume</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>protein_concentration</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>crystal_size_um</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>cryo_protectant</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>crystal_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>screen_name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>temperature_c</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>drop_ratio_protein_to_reservoir</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>reservoir_volume_ul</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>seeding_type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>seed_stock_dilution</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"vapor_diffusion_hanging,vapor_diffusion_sitting,batch,microbatch,lcp,dialysis,free_interface_diffusion"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4262,7 +4826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4313,7 +4877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4369,7 +4933,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4490,7 +5054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4676,7 +5240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4712,6 +5276,128 @@
         </is>
       </c>
       <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>patch_size</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>binning</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dose_weighting</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>bfactor_dose_weighting</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>anisotropic_correction</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>frame_grouping</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_binning</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>drift_total</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>defocus_search_min</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>defocus_search_max</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>defocus_step</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>amplitude_contrast</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>cs_used_in_estimation</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>voltage_used_in_estimation</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -4865,6 +5551,164 @@
       <formula1>"experimental,predicted,inferred,literature,author_statement,curator_inference"</formula1>
     </dataValidation>
   </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>picking_method</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>box_size</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>power_score</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>ncc_score</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>model_file</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>symmetry</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>box_size</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>gold_standard</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>split_strategy</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>resolution_0_143</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>resolution_0_5</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>map_sharpening_bfactor</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>resolution_angstrom</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>fsc_value</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Resolve merge conflicts from main: remove duplicate detector fields
After merging main into detector-refactor branch, resolved duplicate
detector field definitions by keeping our enum-based versions:

- Removed duplicate detector_position (line 585-587 from main)
- Removed duplicate detector_mode (line 588-590 from main)
- Kept our versions with:
  - detector_position: Better description with examples
  - detector_mode: DetectorModeEnum (structured) vs string (free text)

Note: detector_mode appears in two classes intentionally:
- CryoEMInstrument: Default/supported detector mode (capability)
- DataCollectionStrategy: Mode used for specific experiment (setting)

Regenerated all schema artifacts after conflict resolution.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/assets/excel/lambda-ber-schema.xlsx
+++ b/assets/excel/lambda-ber-schema.xlsx
@@ -35,23 +35,30 @@
     <sheet name="Image" sheetId="26" state="visible" r:id="rId26"/>
     <sheet name="Image2D" sheetId="27" state="visible" r:id="rId27"/>
     <sheet name="Image3D" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="FTIRImage" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="FluorescenceImage" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="OpticalImage" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="XRFImage" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="ImageFeature" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="OntologyTerm" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="MolecularComposition" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="BufferComposition" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="StorageConditions" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="CryoEMPreparation" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="CrystallizationConditions" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="XRayPreparation" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="SAXSPreparation" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="ExperimentalConditions" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="DataCollectionStrategy" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="QualityMetrics" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="ComputeResources" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="Movie" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="Micrograph" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="FTIRImage" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="FluorescenceImage" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="OpticalImage" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="XRFImage" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="ImageFeature" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="OntologyTerm" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="MolecularComposition" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="BufferComposition" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="StorageConditions" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="CryoEMPreparation" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="CrystallizationConditions" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="XRayPreparation" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="SAXSPreparation" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="ExperimentalConditions" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="DataCollectionStrategy" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="QualityMetrics" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="ComputeResources" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="MotionCorrectionParameters" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="CTFEstimationParameters" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="ParticlePickingParameters" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="RefinementParameters" sheetId="51" state="visible" r:id="rId51"/>
+    <sheet name="FSCCurve" sheetId="52" state="visible" r:id="rId52"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1891,7 +1898,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:AH1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1957,40 +1964,115 @@
       </c>
       <c r="L1" t="inlineStr">
         <is>
+          <t>cs</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>c2_aperture</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>objective_aperture</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>phase_plate_type</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>energy_filter_present</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>energy_filter_make</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>energy_filter_model</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>energy_filter_slit_width</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>pixel_size_physical</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>microscope_software</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>microscope_software_version</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>spotsize</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>gunlens</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>imaging_mode</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>tem_beam_diameter</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
           <t>instrument_code</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>manufacturer</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>model</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>installation_date</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>current_status</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -2004,7 +2086,7 @@
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"counting,integrating,super_resolution,linear,correlated_double_sampling"</formula1>
     </dataValidation>
-    <dataValidation sqref="P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="AE2:AE1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"operational,maintenance,offline,commissioning"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2251,7 +2333,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AT1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2322,70 +2404,170 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
+          <t>magnification</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>calibrated_pixel_size</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>camera_binning</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>exposure_time_per_frame</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>frames_per_movie</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>total_exposure_time</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>total_dose</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>dose_rate</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>defocus_target</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>defocus_range_min</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>defocus_range_max</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>defocus_range_increment</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>astigmatism_target</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>coma</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>stage_tilt</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>autoloader_slot</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>shots_per_hole</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>holes_per_group</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>acquisition_software</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>acquisition_software_version</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
           <t>wavelength</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>oscillation_angle</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>start_angle</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>number_of_images</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>beam_center_x</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>beam_center_y</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>detector_distance</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>pixel_size_x</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>pixel_size_y</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>total_rotation</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>beamline</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -2413,7 +2595,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BC1"/>
+  <dimension ref="A1:BH1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2679,30 +2861,52 @@
       </c>
       <c r="AZ1" t="inlineStr">
         <is>
+          <t>motion_correction_params</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>ctf_estimation_params</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>particle_picking_params</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>refinement_params</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>fsc_curve</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
           <t>output_files</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"motion_correction,ctf_estimation,particle_picking,classification_2d,classification_3d,refinement,model_building,phasing,integration,scaling,saxs_analysis,em_2d_classification,mass_spec_deconvolution"</formula1>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"molecular_replacement,sad,mad,sir,mir,siras,miras,fragile_mr"</formula1>
     </dataValidation>
@@ -2717,7 +2921,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2763,15 +2967,30 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>storage_uri</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>related_entity</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>file_role</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -2780,10 +2999,10 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"mrc,tiff,hdf5,star,pdb,mmcif,mtz,cbf,cbf_zst,img,h5,ascii,thermo_raw,zip,gz"</formula1>
+      <formula1>"mrc,tiff,hdf5,star,pdb,mmcif,mtz,cbf,cbf_zst,img,h5,ascii,thermo_raw,zip,mrcs,eer,cs,json,csv,ccp4,gz"</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"micrograph,diffraction,scattering,particles,volume,model,metadata,raw_data,processed_data"</formula1>
+      <formula1>"micrograph,diffraction,scattering,particles,volume,model,metadata,raw_data,processed_data,movie,motion_corrected,ctf_estimation,particle_coordinates,class_averages,fsc_curve,map_half,validation_report"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3034,7 +3253,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3045,85 +3264,135 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>wavenumber_min</t>
+          <t>frames</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>wavenumber_max</t>
+          <t>super_resolution</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>spectral_resolution</t>
+          <t>pixel_size_unbinned</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>number_of_scans</t>
+          <t>timestamp</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>apodization_function</t>
+          <t>stage_position_x</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>molecular_signatures</t>
+          <t>stage_position_y</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>background_correction</t>
+          <t>stage_position_z</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>nominal_defocus</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>dose_per_frame</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>beam_shift_x</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>beam_shift_y</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>ice_thickness_estimate</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>grid_square_id</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>hole_id</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>acquisition_group</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>defocus</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>astigmatism</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>file_name</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>acquisition_date</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>pixel_size</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>dimensions_x</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>dimensions_y</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>exposure_time</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>dose</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -3285,7 +3554,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3296,105 +3565,90 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>excitation_wavelength</t>
+          <t>pixel_size</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>emission_wavelength</t>
+          <t>defocus</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>excitation_filter</t>
+          <t>dose</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>emission_filter</t>
+          <t>origin_movie_id</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>fluorophore</t>
+          <t>defocus_u</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>channel_name</t>
+          <t>defocus_v</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>laser_power</t>
+          <t>astigmatism</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>pinhole_size</t>
+          <t>astigmatism_angle</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>quantum_yield</t>
+          <t>resolution_fit_limit</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>defocus</t>
+          <t>ctf_quality_score</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>astigmatism</t>
+          <t>file_name</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>file_name</t>
+          <t>acquisition_date</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>acquisition_date</t>
+          <t>dimensions_x</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>pixel_size</t>
+          <t>dimensions_y</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>dimensions_x</t>
+          <t>exposure_time</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>dimensions_y</t>
+          <t>id</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>exposure_time</t>
+          <t>title</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
-        <is>
-          <t>dose</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -3411,7 +3665,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3422,101 +3676,91 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>illumination_type</t>
+          <t>wavenumber_min</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>magnification</t>
+          <t>wavenumber_max</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>numerical_aperture</t>
+          <t>spectral_resolution</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>color_channels</t>
+          <t>number_of_scans</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>white_balance</t>
+          <t>apodization_function</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>contrast_method</t>
+          <t>molecular_signatures</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>defocus</t>
+          <t>background_correction</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>astigmatism</t>
+          <t>file_name</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>file_name</t>
+          <t>acquisition_date</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>acquisition_date</t>
+          <t>pixel_size</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>pixel_size</t>
+          <t>dimensions_x</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>dimensions_x</t>
+          <t>dimensions_y</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>dimensions_y</t>
+          <t>exposure_time</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>exposure_time</t>
+          <t>dose</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>dose</t>
+          <t>id</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>title</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"brightfield,darkfield,phase_contrast,dic,fluorescence,confocal,polarized,oblique"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3538,6 +3782,248 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>excitation_wavelength</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>emission_wavelength</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>excitation_filter</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>emission_filter</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>fluorophore</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>channel_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>laser_power</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>pinhole_size</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>quantum_yield</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>defocus</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>astigmatism</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>file_name</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>acquisition_date</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>dimensions_x</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>dimensions_y</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>exposure_time</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>dose</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>illumination_type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>magnification</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>numerical_aperture</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>color_channels</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>white_balance</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>contrast_method</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>defocus</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>astigmatism</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>file_name</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>acquisition_date</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>dimensions_x</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>dimensions_y</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>exposure_time</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>dose</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"brightfield,darkfield,phase_contrast,dic,fluorescence,confocal,polarized,oblique"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>beam_energy</t>
         </is>
       </c>
@@ -3655,7 +4141,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3686,7 +4172,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3737,7 +4223,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3778,7 +4264,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3819,7 +4305,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3864,181 +4350,6 @@
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"celsius,kelvin,fahrenheit"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>grid_type</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>support_film</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>hole_size</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>vitrification_method</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>blot_time</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>blot_force</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>humidity_percentage</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>chamber_temperature</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>plasma_treatment</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"c_flat,quantifoil,lacey_carbon,ultrathin_carbon,gold"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"plunge_freezing,high_pressure_freezing,slam_freezing"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:N1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>method</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>crystallization_conditions</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>drop_volume</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>protein_concentration</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>crystal_size_um</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>cryo_protectant</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>crystal_id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>screen_name</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>temperature_c</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>drop_ratio_protein_to_reservoir</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>reservoir_volume_ul</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>seeding_type</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>seed_stock_dilution</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"vapor_diffusion_hanging,vapor_diffusion_sitting,batch,microbatch,lcp,dialysis,free_interface_diffusion"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4148,6 +4459,246 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:W1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>grid_type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>support_film</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>hole_size</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>vitrification_method</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>blot_time</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>blot_force</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>humidity_percentage</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>chamber_temperature</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>grid_material</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>glow_discharge_applied</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>glow_discharge_time</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>glow_discharge_current</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>glow_discharge_atmosphere</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>glow_discharge_pressure</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>vitrification_instrument</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>blot_number</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>wait_time</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>blotter_height</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>blotter_setting</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>sample_applied_volume</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>ethane_temperature</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>plasma_treatment</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"c_flat,quantifoil,lacey_carbon,ultrathin_carbon,gold"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"plunge_freezing,high_pressure_freezing,slam_freezing"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>method</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>crystallization_conditions</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>drop_volume</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>protein_concentration</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>crystal_size_um</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>cryo_protectant</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>crystal_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>screen_name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>temperature_c</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>drop_ratio_protein_to_reservoir</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>reservoir_volume_ul</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>seeding_type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>seed_stock_dilution</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"vapor_diffusion_hanging,vapor_diffusion_sitting,batch,microbatch,lcp,dialysis,free_interface_diffusion"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4298,7 +4849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4349,7 +4900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4405,7 +4956,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4534,7 +5085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4720,7 +5271,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4756,6 +5307,128 @@
         </is>
       </c>
       <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>patch_size</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>binning</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dose_weighting</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>bfactor_dose_weighting</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>anisotropic_correction</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>frame_grouping</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_binning</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>drift_total</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>defocus_search_min</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>defocus_search_max</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>defocus_step</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>amplitude_contrast</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>cs_used_in_estimation</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>voltage_used_in_estimation</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -4909,6 +5582,164 @@
       <formula1>"experimental,predicted,inferred,literature,author_statement,curator_inference"</formula1>
     </dataValidation>
   </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>picking_method</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>box_size</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>power_score</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>ncc_score</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>model_file</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>symmetry</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>box_size</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>gold_standard</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>split_strategy</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>resolution_0_143</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>resolution_0_5</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>map_sharpening_bfactor</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>resolution_angstrom</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>fsc_value</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Replace model_file with three fields for better model tracking
- Add model_name: Name/identifier of the DL model
- Add model_file_path: Path to model file
- Add model_source: Software/source of the model
- Update generated artifacts (JSON schema, GraphQL, OWL, etc.)
- Changes support multiple DL software (Topaz, crYOLO, Warp, etc.)
- Enable better model provenance tracking

Co-authored-by: augeorge <30163079+augeorge@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/assets/excel/lambda-ber-schema.xlsx
+++ b/assets/excel/lambda-ber-schema.xlsx
@@ -5900,7 +5900,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5936,10 +5936,20 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>model_file</t>
+          <t>model_name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
+        <is>
+          <t>model_file_path</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>model_source</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
Remove redundant unit-related slots and enums
Now that all quantitative fields use QuantityValue which includes unit
specification, the following redundant slots are no longer needed:

Removed slots:
- Sample.concentration_unit
- StorageConditions.temperature_unit

Removed enums:
- ConcentrationUnitEnum (no longer needed - units now in QuantityValue)
- TemperatureUnitEnum (no longer needed - units now in QuantityValue)

Updated 12 example files to remove these redundant fields.

This cleanup simplifies the schema and eliminates confusion from having
unit information in two places (both in the enum and in QuantityValue).

All tests passing.

🤖 Generated with Claude Code

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/assets/excel/lambda-ber-schema.xlsx
+++ b/assets/excel/lambda-ber-schema.xlsx
@@ -1618,7 +1618,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH1"/>
+  <dimension ref="A1:AG1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1654,157 +1654,149 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>concentration_unit</t>
+          <t>buffer_composition</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>buffer_composition</t>
+          <t>preparation_method</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>preparation_method</t>
+          <t>storage_conditions</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>storage_conditions</t>
+          <t>organism</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>organism</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>cell_type</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>cell_type</t>
+          <t>parent_sample_id</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>parent_sample_id</t>
+          <t>purity_percentage</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>purity_percentage</t>
+          <t>quality_metrics</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>quality_metrics</t>
+          <t>functional_sites</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>functional_sites</t>
+          <t>structural_features</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>structural_features</t>
+          <t>protein_interactions</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>protein_interactions</t>
+          <t>ligand_interactions</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>ligand_interactions</t>
+          <t>mutation_effects</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>mutation_effects</t>
+          <t>ptm_annotations</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>ptm_annotations</t>
+          <t>biophysical_properties</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>biophysical_properties</t>
+          <t>evolutionary_conservation</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>evolutionary_conservation</t>
+          <t>conformational_ensemble</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
         <is>
-          <t>conformational_ensemble</t>
+          <t>database_cross_references</t>
         </is>
       </c>
       <c r="Y1" t="inlineStr">
         <is>
-          <t>database_cross_references</t>
+          <t>protein_name</t>
         </is>
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>protein_name</t>
+          <t>construct</t>
         </is>
       </c>
       <c r="AA1" t="inlineStr">
         <is>
-          <t>construct</t>
+          <t>tag</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
         <is>
-          <t>tag</t>
+          <t>mutations</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>mutations</t>
+          <t>expression_system</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
         <is>
-          <t>expression_system</t>
+          <t>ligand</t>
         </is>
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>ligand</t>
+          <t>id</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>title</t>
         </is>
       </c>
       <c r="AG1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"protein,nucleic_acid,complex,membrane_protein,virus,organelle"</formula1>
-    </dataValidation>
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"mg_per_ml,micromolar,millimolar,nanomolar"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5011,7 +5003,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5027,31 +5019,21 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>temperature_unit</t>
+          <t>duration</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>duration</t>
+          <t>atmosphere</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
-        <is>
-          <t>atmosphere</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"celsius,kelvin,fahrenheit"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>